<commit_message>
Upload result and Reverse Role Prompt
</commit_message>
<xml_diff>
--- a/outputs/personality_results.xlsx
+++ b/outputs/personality_results.xlsx
@@ -1,40 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoshigi\Desktop\llm-personality\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6CB690-A535-4098-B745-FB8D8FBD3B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B793D61-0D06-4397-8E43-10EF81B467C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="798" firstSheet="5" activeTab="9" xr2:uid="{6FA7EFC1-EF90-415D-8904-9E3DD00F40A1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="798" firstSheet="6" activeTab="11" xr2:uid="{6FA7EFC1-EF90-415D-8904-9E3DD00F40A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="3.5-turbo-AAO-0shot" sheetId="4" r:id="rId1"/>
-    <sheet name="3.5-turbo-SC-0shot" sheetId="6" r:id="rId2"/>
-    <sheet name="3.5-turbo-AAO-Nshot" sheetId="10" r:id="rId3"/>
-    <sheet name="3.5-turbo-SC-Nshot" sheetId="12" r:id="rId4"/>
-    <sheet name="4o-AAO-0Shot" sheetId="7" r:id="rId5"/>
-    <sheet name="4o-SC-0Shot" sheetId="8" r:id="rId6"/>
-    <sheet name="4o-NC-0Shot" sheetId="9" r:id="rId7"/>
-    <sheet name="4o-AAO-Nshot" sheetId="13" r:id="rId8"/>
-    <sheet name="4o-SC-Nshot" sheetId="14" r:id="rId9"/>
-    <sheet name="4o-NC-Nshot" sheetId="15" r:id="rId10"/>
-    <sheet name="INTELLECT" sheetId="16" r:id="rId11"/>
-    <sheet name="CONSCIENTIOUSNESS" sheetId="22" r:id="rId12"/>
-    <sheet name="EXTROVERSION" sheetId="23" r:id="rId13"/>
-    <sheet name="AGREEABLENESS" sheetId="24" r:id="rId14"/>
-    <sheet name="EMOTIONAL_STABILITY" sheetId="25" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="26" r:id="rId1"/>
+    <sheet name="3.5-turbo-AAO-0shot" sheetId="4" r:id="rId2"/>
+    <sheet name="3.5-turbo-SC-0shot" sheetId="6" r:id="rId3"/>
+    <sheet name="3.5-turbo-AAO-Nshot" sheetId="10" r:id="rId4"/>
+    <sheet name="3.5-turbo-SC-Nshot" sheetId="12" r:id="rId5"/>
+    <sheet name="4o-AAO-0Shot" sheetId="7" r:id="rId6"/>
+    <sheet name="4o-SC-0Shot" sheetId="8" r:id="rId7"/>
+    <sheet name="4o-NC-0Shot" sheetId="9" r:id="rId8"/>
+    <sheet name="4o-AAO-Nshot" sheetId="13" r:id="rId9"/>
+    <sheet name="4o-SC-Nshot" sheetId="14" r:id="rId10"/>
+    <sheet name="4o-NC-Nshot" sheetId="15" r:id="rId11"/>
+    <sheet name="INTELLECT" sheetId="16" r:id="rId12"/>
+    <sheet name="CONSCIENTIOUSNESS" sheetId="22" r:id="rId13"/>
+    <sheet name="EXTROVERSION" sheetId="23" r:id="rId14"/>
+    <sheet name="AGREEABLENESS" sheetId="24" r:id="rId15"/>
+    <sheet name="EMOTIONAL_STABILITY" sheetId="25" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="37">
   <si>
     <t>INTELLECT</t>
   </si>
@@ -131,6 +132,40 @@
   </si>
   <si>
     <t>EMOTIONAL_STABILITY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5-turbo-AAO-0shot</t>
+  </si>
+  <si>
+    <t>3.5-turbo-SC-0shot</t>
+  </si>
+  <si>
+    <t>3.5-turbo-AAO-Nshot</t>
+  </si>
+  <si>
+    <t>3.5-turbo-SC-Nshot</t>
+  </si>
+  <si>
+    <t>4o-AAO-0Shot</t>
+  </si>
+  <si>
+    <t>4o-SC-0Shot</t>
+  </si>
+  <si>
+    <t>4o-NC-0Shot</t>
+  </si>
+  <si>
+    <t>4o-AAO-Nshot</t>
+  </si>
+  <si>
+    <t>4o-SC-Nshot</t>
+  </si>
+  <si>
+    <t>4o-NC-Nshot</t>
+  </si>
+  <si>
+    <t>average</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -853,9 +888,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -881,6 +913,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1237,11 +1272,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6568AB-172D-4C3E-B73D-80BF4D630972}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C514626D-EABA-420B-98F2-EBDEF7F2B211}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.4140625" customWidth="1"/>
+    <col min="2" max="2" width="29.9140625" customWidth="1"/>
+    <col min="3" max="3" width="25.25" customWidth="1"/>
+    <col min="4" max="4" width="21.58203125" customWidth="1"/>
+    <col min="5" max="5" width="17.4140625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2">
+        <v>37</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B2:B11)</f>
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:F13" si="0">AVERAGE(C2:C11)</f>
+        <v>31.1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>22.3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>35.1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>20.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61122768-1D64-40B8-9FA5-9DEDEF945F0D}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1255,13 +1556,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1284,33 +1585,33 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3">
-        <v>36</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>39</v>
       </c>
       <c r="E3" s="1">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1">
-        <v>29</v>
-      </c>
-      <c r="G3" s="4">
-        <v>40</v>
+        <v>23</v>
+      </c>
+      <c r="G3" s="7">
+        <v>39</v>
       </c>
       <c r="H3" s="1">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1321,44 +1622,44 @@
         <v>30</v>
       </c>
       <c r="E4" s="5">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1">
-        <v>29</v>
-      </c>
-      <c r="G4" s="7">
-        <v>36</v>
+        <v>12</v>
+      </c>
+      <c r="G4" s="1">
+        <v>31</v>
       </c>
       <c r="H4" s="1">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
-        <v>34</v>
-      </c>
-      <c r="F5" s="5">
-        <v>40</v>
-      </c>
-      <c r="G5" s="7">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3">
+        <v>37</v>
+      </c>
+      <c r="G5" s="4">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1366,23 +1667,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G6" s="5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1390,41 +1691,41 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1">
+        <v>22</v>
+      </c>
+      <c r="G7" s="4">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3">
         <v>29</v>
       </c>
-      <c r="G7" s="4">
-        <v>40</v>
-      </c>
-      <c r="H7" s="3">
-        <v>32</v>
-      </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1">
-        <v>32</v>
-      </c>
-      <c r="G8" s="2">
-        <v>40</v>
+        <v>19</v>
+      </c>
+      <c r="G8" s="1">
+        <v>31</v>
       </c>
       <c r="H8" s="1">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1437,12 +1738,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8209D1B-34A0-4794-AF6B-9E4AD9790BC0}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1456,13 +1757,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1485,7 +1786,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1511,7 +1812,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1535,7 +1836,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1559,7 +1860,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1583,7 +1884,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1908,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1638,258 +1939,258 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62140FCE-BD8A-4458-BE2D-A83E2CCF6560}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="11" width="18.58203125" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="11"/>
+    <col min="1" max="11" width="18.58203125" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>36</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>35</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>38</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>36</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>39</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>39</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>38</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>39</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <v>39</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>35</v>
       </c>
-      <c r="C4" s="12">
-        <v>31</v>
-      </c>
-      <c r="D4" s="12">
-        <v>31</v>
-      </c>
-      <c r="E4" s="12">
-        <v>31</v>
-      </c>
-      <c r="F4" s="12">
-        <v>30</v>
-      </c>
-      <c r="G4" s="12">
+      <c r="C4" s="11">
+        <v>31</v>
+      </c>
+      <c r="D4" s="11">
+        <v>31</v>
+      </c>
+      <c r="E4" s="11">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11">
         <v>28</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>29</v>
       </c>
-      <c r="I4" s="12">
-        <v>30</v>
-      </c>
-      <c r="J4" s="12">
+      <c r="I4" s="11">
+        <v>30</v>
+      </c>
+      <c r="J4" s="11">
         <v>27</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>29</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>26</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>35</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>25</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>29</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>15</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>25</v>
       </c>
-      <c r="I5" s="12">
-        <v>30</v>
-      </c>
-      <c r="J5" s="12">
+      <c r="I5" s="11">
+        <v>30</v>
+      </c>
+      <c r="J5" s="11">
         <v>23</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15">
-        <v>40</v>
-      </c>
-      <c r="C6" s="15">
+      <c r="B6" s="14">
+        <v>40</v>
+      </c>
+      <c r="C6" s="14">
         <v>37</v>
       </c>
-      <c r="D6" s="15">
-        <v>40</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="D6" s="14">
+        <v>40</v>
+      </c>
+      <c r="E6" s="15">
         <v>36</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>37</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>38</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>39</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="16">
         <v>37</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="15">
         <v>39</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="15">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="12">
-        <v>31</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="11">
+        <v>31</v>
+      </c>
+      <c r="C7" s="11">
         <v>24</v>
       </c>
-      <c r="D7" s="12">
-        <v>31</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="11">
+        <v>31</v>
+      </c>
+      <c r="E7" s="11">
         <v>23</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>13</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>9</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>18</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>13</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>12</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>20</v>
       </c>
     </row>
@@ -1899,11 +2200,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA47CE27-10AF-4A8B-864B-597DFCDD9EA8}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1912,242 +2213,242 @@
     <col min="1" max="11" width="18.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="12" t="s">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12">
-        <v>30</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="11">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11">
         <v>32</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>33</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>33</v>
       </c>
-      <c r="F3" s="12">
-        <v>30</v>
-      </c>
-      <c r="G3" s="12">
-        <v>31</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="F3" s="11">
+        <v>30</v>
+      </c>
+      <c r="G3" s="11">
+        <v>31</v>
+      </c>
+      <c r="H3" s="11">
         <v>33</v>
       </c>
-      <c r="I3" s="12">
-        <v>30</v>
-      </c>
-      <c r="J3" s="12">
-        <v>30</v>
-      </c>
-      <c r="K3" s="12">
+      <c r="I3" s="11">
+        <v>30</v>
+      </c>
+      <c r="J3" s="11">
+        <v>30</v>
+      </c>
+      <c r="K3" s="11">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>36</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>37</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>38</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>37</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>35</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>38</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>37</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <v>36</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>38</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>29</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>22</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>29</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>23</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>19</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>11</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>16</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>19</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>12</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>36</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>37</v>
       </c>
-      <c r="D6" s="15">
-        <v>40</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="D6" s="14">
+        <v>40</v>
+      </c>
+      <c r="E6" s="15">
         <v>37</v>
       </c>
-      <c r="F6" s="12">
-        <v>31</v>
-      </c>
-      <c r="G6" s="16">
+      <c r="F6" s="11">
+        <v>31</v>
+      </c>
+      <c r="G6" s="15">
         <v>38</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <v>36</v>
       </c>
-      <c r="I6" s="12">
-        <v>30</v>
-      </c>
-      <c r="J6" s="12">
-        <v>31</v>
-      </c>
-      <c r="K6" s="12">
+      <c r="I6" s="11">
+        <v>30</v>
+      </c>
+      <c r="J6" s="11">
+        <v>31</v>
+      </c>
+      <c r="K6" s="11">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>28</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>28</v>
       </c>
-      <c r="D7" s="12">
-        <v>30</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="11">
+        <v>30</v>
+      </c>
+      <c r="E7" s="11">
         <v>28</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>20</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>19</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>20</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>12</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>19</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>17</v>
       </c>
     </row>
@@ -2157,11 +2458,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C8C73B-3C2E-4F1B-94C8-03EF69B9440F}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
@@ -2170,242 +2471,242 @@
     <col min="1" max="11" width="18.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="12" t="s">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>32</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>35</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>32</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>35</v>
       </c>
-      <c r="F3" s="12">
-        <v>31</v>
-      </c>
-      <c r="G3" s="12">
-        <v>31</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="F3" s="11">
+        <v>31</v>
+      </c>
+      <c r="G3" s="11">
+        <v>31</v>
+      </c>
+      <c r="H3" s="11">
         <v>35</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>35</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>36</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>34</v>
       </c>
-      <c r="C4" s="12">
-        <v>31</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="C4" s="11">
+        <v>31</v>
+      </c>
+      <c r="D4" s="11">
         <v>34</v>
       </c>
-      <c r="E4" s="12">
-        <v>31</v>
-      </c>
-      <c r="F4" s="12">
-        <v>30</v>
-      </c>
-      <c r="G4" s="12">
-        <v>30</v>
-      </c>
-      <c r="H4" s="12">
-        <v>30</v>
-      </c>
-      <c r="I4" s="12">
-        <v>30</v>
-      </c>
-      <c r="J4" s="12">
-        <v>30</v>
-      </c>
-      <c r="K4" s="12">
+      <c r="E4" s="11">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11">
+        <v>30</v>
+      </c>
+      <c r="H4" s="11">
+        <v>30</v>
+      </c>
+      <c r="I4" s="11">
+        <v>30</v>
+      </c>
+      <c r="J4" s="11">
+        <v>30</v>
+      </c>
+      <c r="K4" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="14">
-        <v>40</v>
-      </c>
-      <c r="C5" s="13">
+      <c r="B5" s="13">
+        <v>40</v>
+      </c>
+      <c r="C5" s="12">
         <v>35</v>
       </c>
-      <c r="D5" s="14">
-        <v>40</v>
-      </c>
-      <c r="E5" s="13">
+      <c r="D5" s="13">
+        <v>40</v>
+      </c>
+      <c r="E5" s="12">
         <v>35</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>35</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>37</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>37</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>35</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>37</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16">
-        <v>40</v>
-      </c>
-      <c r="C6" s="15">
-        <v>40</v>
-      </c>
-      <c r="D6" s="16">
-        <v>40</v>
-      </c>
-      <c r="E6" s="15">
-        <v>40</v>
-      </c>
-      <c r="F6" s="15">
-        <v>40</v>
-      </c>
-      <c r="G6" s="15">
-        <v>40</v>
-      </c>
-      <c r="H6" s="15">
-        <v>40</v>
-      </c>
-      <c r="I6" s="15">
-        <v>40</v>
-      </c>
-      <c r="J6" s="15">
-        <v>40</v>
-      </c>
-      <c r="K6" s="15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15">
+        <v>40</v>
+      </c>
+      <c r="C6" s="14">
+        <v>40</v>
+      </c>
+      <c r="D6" s="15">
+        <v>40</v>
+      </c>
+      <c r="E6" s="14">
+        <v>40</v>
+      </c>
+      <c r="F6" s="14">
+        <v>40</v>
+      </c>
+      <c r="G6" s="14">
+        <v>40</v>
+      </c>
+      <c r="H6" s="14">
+        <v>40</v>
+      </c>
+      <c r="I6" s="14">
+        <v>40</v>
+      </c>
+      <c r="J6" s="14">
+        <v>40</v>
+      </c>
+      <c r="K6" s="14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
-        <v>30</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="11">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11">
         <v>27</v>
       </c>
-      <c r="D7" s="12">
-        <v>30</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="D7" s="11">
+        <v>30</v>
+      </c>
+      <c r="E7" s="11">
         <v>27</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>23</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>22</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>26</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>13</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>23</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>20</v>
       </c>
     </row>
@@ -2415,11 +2716,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB1BA14-7DFA-4B2C-A036-80CDC78DDE2C}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
@@ -2428,242 +2729,242 @@
     <col min="1" max="11" width="18.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>36</v>
       </c>
-      <c r="C3" s="12">
-        <v>30</v>
-      </c>
-      <c r="D3" s="12">
+      <c r="C3" s="11">
+        <v>30</v>
+      </c>
+      <c r="D3" s="11">
         <v>36</v>
       </c>
-      <c r="E3" s="12">
-        <v>30</v>
-      </c>
-      <c r="F3" s="12">
-        <v>30</v>
-      </c>
-      <c r="G3" s="12">
-        <v>31</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="E3" s="11">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11">
+        <v>30</v>
+      </c>
+      <c r="G3" s="11">
+        <v>31</v>
+      </c>
+      <c r="H3" s="11">
         <v>33</v>
       </c>
-      <c r="I3" s="12">
-        <v>30</v>
-      </c>
-      <c r="J3" s="12">
+      <c r="I3" s="11">
+        <v>30</v>
+      </c>
+      <c r="J3" s="11">
         <v>29</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>35</v>
       </c>
-      <c r="C4" s="12">
-        <v>31</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="C4" s="11">
+        <v>31</v>
+      </c>
+      <c r="D4" s="11">
         <v>36</v>
       </c>
-      <c r="E4" s="12">
-        <v>31</v>
-      </c>
-      <c r="F4" s="12">
-        <v>30</v>
-      </c>
-      <c r="G4" s="12">
-        <v>31</v>
-      </c>
-      <c r="H4" s="12">
-        <v>31</v>
-      </c>
-      <c r="I4" s="12">
-        <v>30</v>
-      </c>
-      <c r="J4" s="12">
+      <c r="E4" s="11">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11">
+        <v>31</v>
+      </c>
+      <c r="H4" s="11">
+        <v>31</v>
+      </c>
+      <c r="I4" s="11">
+        <v>30</v>
+      </c>
+      <c r="J4" s="11">
         <v>29</v>
       </c>
-      <c r="K4" s="12">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>29</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>22</v>
       </c>
-      <c r="D5" s="12">
-        <v>30</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="D5" s="11">
+        <v>30</v>
+      </c>
+      <c r="E5" s="11">
         <v>21</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>21</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>21</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>21</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>23</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>16</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="14">
-        <v>40</v>
-      </c>
-      <c r="C6" s="14">
-        <v>40</v>
-      </c>
-      <c r="D6" s="14">
-        <v>40</v>
-      </c>
-      <c r="E6" s="14">
-        <v>40</v>
-      </c>
-      <c r="F6" s="14">
-        <v>40</v>
-      </c>
-      <c r="G6" s="14">
-        <v>40</v>
-      </c>
-      <c r="H6" s="14">
-        <v>40</v>
-      </c>
-      <c r="I6" s="14">
-        <v>40</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="B6" s="13">
+        <v>40</v>
+      </c>
+      <c r="C6" s="13">
+        <v>40</v>
+      </c>
+      <c r="D6" s="13">
+        <v>40</v>
+      </c>
+      <c r="E6" s="13">
+        <v>40</v>
+      </c>
+      <c r="F6" s="13">
+        <v>40</v>
+      </c>
+      <c r="G6" s="13">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13">
+        <v>40</v>
+      </c>
+      <c r="I6" s="13">
+        <v>40</v>
+      </c>
+      <c r="J6" s="13">
         <v>39</v>
       </c>
-      <c r="K6" s="14">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
-        <v>31</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="11">
+        <v>31</v>
+      </c>
+      <c r="C7" s="11">
         <v>29</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>32</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>28</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>13</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>23</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>26</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>20</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>23</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>21</v>
       </c>
     </row>
@@ -2673,11 +2974,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F28D72-AF0C-48B2-B255-89D89C2E7A7D}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2686,242 +2987,242 @@
     <col min="1" max="11" width="18.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="H2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>36</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>33</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>36</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>32</v>
       </c>
-      <c r="F3" s="12">
-        <v>30</v>
-      </c>
-      <c r="G3" s="12">
-        <v>31</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="F3" s="11">
+        <v>30</v>
+      </c>
+      <c r="G3" s="11">
+        <v>31</v>
+      </c>
+      <c r="H3" s="11">
         <v>35</v>
       </c>
-      <c r="I3" s="12">
-        <v>30</v>
-      </c>
-      <c r="J3" s="12">
+      <c r="I3" s="11">
+        <v>30</v>
+      </c>
+      <c r="J3" s="11">
         <v>32</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>36</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>32</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>39</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>32</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>36</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <v>36</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>36</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>37</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <v>37</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>29</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>22</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>28</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>22</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>28</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>15</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>20</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>29</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>22</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="15">
-        <v>40</v>
-      </c>
-      <c r="C6" s="15">
+      <c r="B6" s="14">
+        <v>40</v>
+      </c>
+      <c r="C6" s="14">
         <v>38</v>
       </c>
-      <c r="D6" s="15">
-        <v>40</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="D6" s="14">
+        <v>40</v>
+      </c>
+      <c r="E6" s="14">
         <v>37</v>
       </c>
-      <c r="F6" s="12">
-        <v>31</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="F6" s="11">
+        <v>31</v>
+      </c>
+      <c r="G6" s="11">
         <v>35</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <v>39</v>
       </c>
-      <c r="I6" s="12">
-        <v>31</v>
-      </c>
-      <c r="J6" s="15">
-        <v>40</v>
-      </c>
-      <c r="K6" s="16">
+      <c r="I6" s="11">
+        <v>31</v>
+      </c>
+      <c r="J6" s="14">
+        <v>40</v>
+      </c>
+      <c r="K6" s="15">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>32</v>
       </c>
-      <c r="C7" s="13">
-        <v>31</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="C7" s="12">
+        <v>31</v>
+      </c>
+      <c r="D7" s="12">
         <v>33</v>
       </c>
-      <c r="E7" s="13">
-        <v>30</v>
-      </c>
-      <c r="F7" s="14">
-        <v>40</v>
-      </c>
-      <c r="G7" s="13">
-        <v>30</v>
-      </c>
-      <c r="H7" s="14">
-        <v>40</v>
-      </c>
-      <c r="I7" s="14">
-        <v>40</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="E7" s="12">
+        <v>30</v>
+      </c>
+      <c r="F7" s="13">
+        <v>40</v>
+      </c>
+      <c r="G7" s="12">
+        <v>30</v>
+      </c>
+      <c r="H7" s="13">
+        <v>40</v>
+      </c>
+      <c r="I7" s="13">
+        <v>40</v>
+      </c>
+      <c r="J7" s="12">
         <v>29</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <v>39</v>
       </c>
     </row>
@@ -2932,11 +3233,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DB95F7-D6B6-4C1F-842F-ABEC44D76D5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6568AB-172D-4C3E-B73D-80BF4D630972}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+      <selection activeCell="D2" sqref="D2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2950,13 +3251,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2979,7 +3280,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2989,23 +3290,23 @@
         <v>9</v>
       </c>
       <c r="D3" s="3">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1">
         <v>35</v>
       </c>
-      <c r="E3" s="1">
-        <v>31</v>
-      </c>
       <c r="F3" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3" s="4">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3013,47 +3314,47 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" s="5">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3">
-        <v>35</v>
-      </c>
-      <c r="G5" s="4">
+        <v>34</v>
+      </c>
+      <c r="F5" s="5">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3061,23 +3362,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5">
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3085,41 +3386,41 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3">
         <v>32</v>
       </c>
-      <c r="F7" s="1">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4">
-        <v>38</v>
-      </c>
-      <c r="H7" s="3">
-        <v>31</v>
-      </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H8" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3133,11 +3434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1C7D2C-FE85-41C2-B400-1FB97FC0B72D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DB95F7-D6B6-4C1F-842F-ABEC44D76D5F}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3151,13 +3452,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3180,7 +3481,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3190,71 +3491,71 @@
         <v>9</v>
       </c>
       <c r="D3" s="3">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1">
         <v>31</v>
       </c>
       <c r="F3" s="1">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G3" s="4">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>33</v>
-      </c>
-      <c r="E4" s="3">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="E4" s="5">
+        <v>37</v>
       </c>
       <c r="F4" s="1">
-        <v>29</v>
-      </c>
-      <c r="G4" s="4">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="G4" s="7">
+        <v>37</v>
       </c>
       <c r="H4" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
-        <v>34</v>
-      </c>
-      <c r="F5" s="5">
-        <v>40</v>
-      </c>
-      <c r="G5" s="7">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3">
+        <v>35</v>
+      </c>
+      <c r="G5" s="4">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3262,23 +3563,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5">
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3286,41 +3587,41 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H7" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
         <v>37</v>
       </c>
-      <c r="E8" s="1">
-        <v>37</v>
-      </c>
-      <c r="F8" s="1">
-        <v>32</v>
-      </c>
-      <c r="G8" s="2">
-        <v>40</v>
-      </c>
       <c r="H8" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3330,16 +3631,15 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF14EFC7-4DEB-4ADF-99DE-7BBDDC7D5B38}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1C7D2C-FE85-41C2-B400-1FB97FC0B72D}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3353,13 +3653,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3382,81 +3682,81 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>38</v>
       </c>
       <c r="E3" s="1">
         <v>31</v>
       </c>
       <c r="F3" s="1">
-        <v>25</v>
-      </c>
-      <c r="G3" s="7">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="G3" s="4">
+        <v>40</v>
       </c>
       <c r="H3" s="1">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>33</v>
       </c>
-      <c r="E4" s="5">
-        <v>37</v>
+      <c r="E4" s="3">
+        <v>38</v>
       </c>
       <c r="F4" s="1">
-        <v>23</v>
-      </c>
-      <c r="G4" s="7">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="G4" s="4">
+        <v>40</v>
       </c>
       <c r="H4" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3">
-        <v>35</v>
-      </c>
-      <c r="G5" s="4">
+        <v>34</v>
+      </c>
+      <c r="F5" s="5">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3464,23 +3764,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G6" s="5">
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3488,41 +3788,41 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="4">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H7" s="3">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H8" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3532,15 +3832,16 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA6D359-2D0B-450C-AE37-1B2953C2DBA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF14EFC7-4DEB-4ADF-99DE-7BBDDC7D5B38}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H8"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3554,13 +3855,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3583,7 +3884,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3593,23 +3894,23 @@
         <v>10</v>
       </c>
       <c r="D3" s="5">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="G3" s="7">
+        <v>36</v>
       </c>
       <c r="H3" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3617,23 +3918,23 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="7">
+        <v>37</v>
       </c>
       <c r="H4" s="1">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3641,10 +3942,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" s="3">
         <v>35</v>
@@ -3653,11 +3954,11 @@
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3668,7 +3969,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1">
         <v>21</v>
@@ -3677,53 +3978,53 @@
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1">
-        <v>28</v>
-      </c>
-      <c r="G7" s="1">
-        <v>31</v>
-      </c>
-      <c r="H7" s="5">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="G7" s="4">
+        <v>37</v>
+      </c>
+      <c r="H7" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
         <v>37</v>
       </c>
-      <c r="E8" s="1">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1">
-        <v>34</v>
-      </c>
       <c r="H8" s="1">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3737,11 +4038,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF616E7-BB7A-422A-B5BC-E66B47C0DFC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA6D359-2D0B-450C-AE37-1B2953C2DBA4}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3755,13 +4056,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3784,7 +4085,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3797,20 +4098,20 @@
         <v>39</v>
       </c>
       <c r="E3" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
-        <v>15</v>
-      </c>
-      <c r="G3" s="6">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="G3" s="1">
+        <v>37</v>
       </c>
       <c r="H3" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3818,23 +4119,23 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="5">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7">
-        <v>38</v>
+        <v>19</v>
+      </c>
+      <c r="G4" s="1">
+        <v>31</v>
       </c>
       <c r="H4" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3848,17 +4149,17 @@
         <v>30</v>
       </c>
       <c r="F5" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3866,10 +4167,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
         <v>21</v>
@@ -3878,53 +4179,53 @@
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1">
         <v>36</v>
       </c>
       <c r="F7" s="1">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6">
-        <v>35</v>
-      </c>
-      <c r="H7" s="3">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="G7" s="1">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3938,11 +4239,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1260BA8-E8C0-4D46-95E1-711DFF934207}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF616E7-BB7A-422A-B5BC-E66B47C0DFC7}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3956,13 +4257,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -3985,33 +4286,33 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1">
-        <v>25</v>
-      </c>
-      <c r="G3" s="4">
-        <v>39</v>
-      </c>
-      <c r="H3" s="1">
-        <v>18</v>
-      </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4019,23 +4320,23 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="5">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="7">
+        <v>38</v>
       </c>
       <c r="H4" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4043,7 +4344,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1">
         <v>30</v>
@@ -4055,11 +4356,11 @@
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4067,7 +4368,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1">
         <v>31</v>
@@ -4079,53 +4380,53 @@
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1">
+        <v>31</v>
+      </c>
+      <c r="E7" s="4">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6">
         <v>35</v>
       </c>
-      <c r="E7" s="1">
-        <v>36</v>
-      </c>
-      <c r="F7" s="1">
-        <v>20</v>
-      </c>
-      <c r="G7" s="1">
-        <v>39</v>
-      </c>
-      <c r="H7" s="5">
-        <v>40</v>
+      <c r="H7" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4139,11 +4440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F6908B-7206-4724-8D04-85BFF788B28F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1260BA8-E8C0-4D46-95E1-711DFF934207}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4157,13 +4458,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4186,33 +4487,33 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4">
         <v>39</v>
       </c>
-      <c r="E3" s="1">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1">
-        <v>30</v>
-      </c>
-      <c r="G3" s="9">
-        <v>37</v>
-      </c>
       <c r="H3" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4220,23 +4521,23 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1">
         <v>36</v>
       </c>
-      <c r="F4" s="1">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1">
-        <v>30</v>
-      </c>
       <c r="H4" s="1">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4250,17 +4551,17 @@
         <v>30</v>
       </c>
       <c r="F5" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5" s="4">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4268,23 +4569,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="5">
         <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4292,41 +4593,41 @@
         <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H7" s="5">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1">
         <v>30</v>
       </c>
       <c r="F8" s="1">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -4340,11 +4641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61122768-1D64-40B8-9FA5-9DEDEF945F0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F6908B-7206-4724-8D04-85BFF788B28F}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+      <selection activeCell="D8" sqref="D8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4358,13 +4659,13 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4387,7 +4688,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4400,20 +4701,20 @@
         <v>39</v>
       </c>
       <c r="E3" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
-        <v>23</v>
-      </c>
-      <c r="G3" s="7">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="G3" s="8">
+        <v>37</v>
       </c>
       <c r="H3" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4424,20 +4725,20 @@
         <v>30</v>
       </c>
       <c r="E4" s="5">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1">
         <v>12</v>
       </c>
-      <c r="G4" s="1">
-        <v>31</v>
-      </c>
-      <c r="H4" s="1">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4445,23 +4746,23 @@
         <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
         <v>30</v>
       </c>
       <c r="F5" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4">
         <v>40</v>
       </c>
       <c r="H5" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4469,65 +4770,65 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>37</v>
       </c>
       <c r="F7" s="1">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4">
-        <v>40</v>
-      </c>
-      <c r="H7" s="3">
         <v>29</v>
       </c>
+      <c r="G7" s="1">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>